<commit_message>
Added first period guide
</commit_message>
<xml_diff>
--- a/Parcial 1/Clases/03/Estilos de graficas.xlsx
+++ b/Parcial 1/Clases/03/Estilos de graficas.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hca\Desktop\hcp-repo\Parcial 1\Clases\03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmond\Documents\ITAM\Semestre 10\Herramientas Computacionales para Produccion Empresarial\hcp-repo\Parcial 1\Clases\03\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7725" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7725" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Ejercicio de graficos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>hca</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -268,7 +268,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -750,7 +750,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="281403152"/>
@@ -808,7 +808,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="281402168"/>
@@ -825,7 +825,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -851,7 +850,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -881,7 +880,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -932,7 +931,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -958,7 +956,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1011,7 +1009,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-MX"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1024,7 +1022,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1070,16 +1067,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>96</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1137,7 +1134,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1163,7 +1159,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-MX"/>
+              <a:endParaRPr lang="es-ES"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1201,7 +1197,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="526466304"/>
@@ -1257,7 +1253,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="526468272"/>
@@ -1310,7 +1306,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1362,7 +1358,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1388,7 +1383,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1466,7 +1461,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-MX"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1479,7 +1474,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1525,16 +1519,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>96</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1607,7 +1601,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="526466304"/>
@@ -1652,7 +1646,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="526468272"/>
@@ -1711,7 +1705,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1761,7 +1755,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1817,7 +1811,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -1851,7 +1844,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1979,16 +1972,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2057,16 +2050,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2135,16 +2128,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2204,7 +2197,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="594515272"/>
@@ -2260,7 +2253,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="594515928"/>
@@ -2277,7 +2270,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -2307,7 +2299,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2335,7 +2327,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2386,7 +2378,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -2420,7 +2411,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2503,16 +2494,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2591,16 +2582,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2675,16 +2666,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2754,7 +2745,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2777,7 +2767,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-MX"/>
+              <a:endParaRPr lang="es-ES"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2815,7 +2805,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="538161680"/>
@@ -2871,7 +2861,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="538160696"/>
@@ -2931,7 +2921,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2960,7 +2950,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3016,7 +3006,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3042,7 +3031,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3120,16 +3109,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>619750</c:v>
+                  <c:v>1320790</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>831550</c:v>
+                  <c:v>786540</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>305190</c:v>
+                  <c:v>620200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1231240</c:v>
+                  <c:v>1433260</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3195,16 +3184,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>460449.20000000007</c:v>
+                  <c:v>1011204</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>634341.80000000005</c:v>
+                  <c:v>576238.80000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>227346</c:v>
+                  <c:v>471711.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>907743.60000000009</c:v>
+                  <c:v>1087726.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3284,7 +3273,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-MX"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -3296,7 +3285,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3322,16 +3310,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>159300.79999999993</c:v>
+                  <c:v>309586</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>197208.19999999995</c:v>
+                  <c:v>210301.19999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77844</c:v>
+                  <c:v>148488.59999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>323496.39999999991</c:v>
+                  <c:v>345533.19999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3392,7 +3380,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="675819656"/>
@@ -3448,7 +3436,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="675822936"/>
@@ -3471,7 +3459,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3499,7 +3486,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3526,7 +3513,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3552,7 +3539,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3578,7 +3564,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3712,16 +3698,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1549.375</c:v>
+                  <c:v>3301.9749999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2078.875</c:v>
+                  <c:v>1966.3500000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>762.97500000000002</c:v>
+                  <c:v>1550.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3078.1</c:v>
+                  <c:v>3583.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3816,16 +3802,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>111555</c:v>
+                  <c:v>237742.19999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>149679</c:v>
+                  <c:v>141577.19999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54934.2</c:v>
+                  <c:v>111636</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>221623.19999999998</c:v>
+                  <c:v>257986.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3884,7 +3870,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="526456464"/>
@@ -3943,7 +3929,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="526460728"/>
@@ -3960,7 +3946,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3986,7 +3971,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4016,7 +4001,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7827,7 +7812,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7862,7 +7853,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1" title="UNIDADES VENDIDAS"/>
+        <xdr:cNvPr id="2" name="Gráfico 1" title="UNIDADES VENDIDAS">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7892,7 +7889,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Gráfico 5" title="UNIDADES VENDIDAS"/>
+        <xdr:cNvPr id="6" name="Gráfico 5" title="UNIDADES VENDIDAS">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -7924,7 +7927,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Gráfico 7"/>
+        <xdr:cNvPr id="8" name="Gráfico 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7954,7 +7963,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Gráfico 8"/>
+        <xdr:cNvPr id="9" name="Gráfico 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7984,7 +7999,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Gráfico 9"/>
+        <xdr:cNvPr id="10" name="Gráfico 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8014,7 +8035,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Gráfico 10"/>
+        <xdr:cNvPr id="11" name="Gráfico 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8546,19 +8573,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -8569,7 +8596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>0</v>
       </c>
@@ -8581,7 +8608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>0.1</v>
       </c>
@@ -8590,7 +8617,7 @@
         <v>-3.7918861169915807</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>0.2</v>
       </c>
@@ -8599,7 +8626,7 @@
         <v>-3.6763932022500212</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>0.3</v>
       </c>
@@ -8608,7 +8635,7 @@
         <v>-3.5761387212474167</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>0.4</v>
       </c>
@@ -8617,7 +8644,7 @@
         <v>-3.4837722339831618</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>0.5</v>
       </c>
@@ -8626,7 +8653,7 @@
         <v>-3.396446609406726</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>0.6</v>
       </c>
@@ -8635,7 +8662,7 @@
         <v>-3.3127016653792585</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>0.7</v>
       </c>
@@ -8644,7 +8671,7 @@
         <v>-3.2316699867329621</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>0.8</v>
       </c>
@@ -8653,7 +8680,7 @@
         <v>-3.1527864045000422</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>0.9</v>
       </c>
@@ -8662,7 +8689,7 @@
         <v>-3.0756583509747433</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1</v>
       </c>
@@ -8671,7 +8698,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>1.1000000000000001</v>
       </c>
@@ -8680,7 +8707,7 @@
         <v>-2.9255955759149241</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>1.2</v>
       </c>
@@ -8689,7 +8716,7 @@
         <v>-2.8522774424948341</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>1.3</v>
       </c>
@@ -8698,7 +8725,7 @@
         <v>-2.779912287450431</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>1.4</v>
       </c>
@@ -8707,7 +8734,7 @@
         <v>-2.7083920216900386</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>1.5</v>
       </c>
@@ -8716,7 +8743,7 @@
         <v>-2.6376275643042053</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>1.6</v>
       </c>
@@ -8725,7 +8752,7 @@
         <v>-2.5675444679663242</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>1.7</v>
       </c>
@@ -8734,7 +8761,7 @@
         <v>-2.4980797594797353</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>1.8</v>
       </c>
@@ -8743,7 +8770,7 @@
         <v>-2.4291796067500631</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>1.9</v>
       </c>
@@ -8752,7 +8779,7 @@
         <v>-2.3607975623954891</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>2</v>
       </c>
@@ -8761,7 +8788,7 @@
         <v>-2.2928932188134525</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>2.1</v>
       </c>
@@ -8770,7 +8797,7 @@
         <v>-2.2254311626905281</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>2.2000000000000002</v>
       </c>
@@ -8779,7 +8806,7 @@
         <v>-2.1583801512904337</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>2.2999999999999998</v>
       </c>
@@ -8788,7 +8815,7 @@
         <v>-2.0917124555948452</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>2.4</v>
       </c>
@@ -8797,7 +8824,7 @@
         <v>-2.0254033307585164</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>2.5</v>
       </c>
@@ -8806,7 +8833,7 @@
         <v>-1.959430584957905</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>2.6</v>
       </c>
@@ -8815,7 +8842,7 @@
         <v>-1.8937742251701448</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>2.7</v>
       </c>
@@ -8824,7 +8851,7 @@
         <v>-1.8284161637422507</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>2.8</v>
       </c>
@@ -8833,7 +8860,7 @@
         <v>-1.7633399734659245</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>2.9</v>
       </c>
@@ -8842,7 +8869,7 @@
         <v>-1.69853068170368</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>3</v>
       </c>
@@ -8851,7 +8878,7 @@
         <v>-1.6339745962155614</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>3.1</v>
       </c>
@@ -8860,7 +8887,7 @@
         <v>-1.5696591569170495</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>3.2</v>
       </c>
@@ -8869,7 +8896,7 @@
         <v>-1.5055728090000842</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>3.3</v>
       </c>
@@ -8878,7 +8905,7 @@
         <v>-1.4417048937707526</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>3.4</v>
       </c>
@@ -8887,7 +8914,7 @@
         <v>-1.3780455542707113</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>3.5</v>
       </c>
@@ -8896,7 +8923,7 @@
         <v>-1.3145856533065148</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>3.6</v>
       </c>
@@ -8905,7 +8932,7 @@
         <v>-1.2513167019494862</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>3.7</v>
       </c>
@@ -8914,7 +8941,7 @@
         <v>-1.1882307969164327</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>3.8</v>
       </c>
@@ -8923,7 +8950,7 @@
         <v>-1.1253205655191039</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>3.9</v>
       </c>
@@ -8932,7 +8959,7 @@
         <v>-1.0625791170934251</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>4</v>
       </c>
@@ -8941,7 +8968,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>4.0999999999999996</v>
       </c>
@@ -8950,7 +8977,7 @@
         <v>-0.96242283656582917</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>4.2</v>
       </c>
@@ -8959,7 +8986,7 @@
         <v>-0.92469507659595962</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>4.3</v>
       </c>
@@ -8968,7 +8995,7 @@
         <v>-0.88682206766638583</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>4.4000000000000004</v>
       </c>
@@ -8977,7 +9004,7 @@
         <v>-0.84880884817015145</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>4.5</v>
       </c>
@@ -8986,7 +9013,7 @@
         <v>-0.81066017177982097</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>4.5999999999999996</v>
       </c>
@@ -8995,7 +9022,7 @@
         <v>-0.77238052947636104</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>4.7</v>
       </c>
@@ -9004,7 +9031,7 @@
         <v>-0.73397416943393967</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>4.8</v>
       </c>
@@ -9013,7 +9040,7 @@
         <v>-0.69544511501033224</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>4.9000000000000004</v>
       </c>
@@ -9022,7 +9049,7 @@
         <v>-0.65679718105893237</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>5</v>
       </c>
@@ -9031,7 +9058,7 @@
         <v>-0.6180339887498949</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>5.0999999999999996</v>
       </c>
@@ -9040,7 +9067,7 @@
         <v>-0.57915897906362179</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>5.2</v>
       </c>
@@ -9049,7 +9076,7 @@
         <v>-0.54017542509913774</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>5.3</v>
       </c>
@@ -9058,7 +9085,7 @@
         <v>-0.50108644332213359</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>5.4</v>
       </c>
@@ -9067,7 +9094,7 @@
         <v>-0.46189500386222493</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>5.5</v>
       </c>
@@ -9076,7 +9103,7 @@
         <v>-0.42260393995585765</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>5.6</v>
       </c>
@@ -9085,7 +9112,7 @@
         <v>-0.38321595661992358</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>5.7</v>
       </c>
@@ -9094,7 +9121,7 @@
         <v>-0.34373363863133211</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>5.8</v>
       </c>
@@ -9103,7 +9130,7 @@
         <v>-0.30415945787922993</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>5.9</v>
       </c>
@@ -9112,7 +9139,7 @@
         <v>-0.26449578014911168</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>6</v>
       </c>
@@ -9121,7 +9148,7 @@
         <v>-0.22474487139158894</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>6.1</v>
       </c>
@@ -9130,7 +9157,7 @@
         <v>-0.18490890352284683</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>6.2</v>
       </c>
@@ -9139,7 +9166,7 @@
         <v>-0.14498995979887308</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>6.3</v>
       </c>
@@ -9148,7 +9175,7 @@
         <v>-0.10499003980111343</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>6.4</v>
       </c>
@@ -9157,7 +9184,7 @@
         <v>-6.4911064067351809E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>6.5</v>
       </c>
@@ -9166,7 +9193,7 @@
         <v>-2.4754878398196123E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>6.6</v>
       </c>
@@ -9175,7 +9202,7 @@
         <v>1.5476742133486709E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>6.7</v>
       </c>
@@ -9184,7 +9211,7 @@
         <v>5.5782089445521876E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>6.8</v>
       </c>
@@ -9193,7 +9220,7 @@
         <v>9.6159518959470169E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>6.9</v>
       </c>
@@ -9202,7 +9229,7 @@
         <v>0.1366074463436302</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>7</v>
       </c>
@@ -9211,7 +9238,7 @@
         <v>0.17712434446770464</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>7.1</v>
       </c>
@@ -9220,7 +9247,7 @@
         <v>0.21770874055257705</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>7.2</v>
       </c>
@@ -9229,7 +9256,7 @@
         <v>0.25835921350012647</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>7.3</v>
       </c>
@@ -9238,7 +9265,7 @@
         <v>0.29907439138937031</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>7.4</v>
       </c>
@@ -9247,7 +9274,7 @@
         <v>0.33985294912645614</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>7.5</v>
       </c>
@@ -9256,7 +9283,7 @@
         <v>0.38069360623708448</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>7.6</v>
       </c>
@@ -9265,7 +9292,7 @@
         <v>0.42159512479097749</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>7.7</v>
       </c>
@@ -9274,7 +9301,7 @@
         <v>0.46255630744883902</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>7.8</v>
       </c>
@@ -9283,7 +9310,7 @@
         <v>0.50357599562310584</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>7.9</v>
       </c>
@@ -9292,7 +9319,7 @@
         <v>0.54465306774448052</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>8</v>
       </c>
@@ -9301,7 +9328,7 @@
         <v>0.58578643762690508</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>8.1</v>
       </c>
@@ -9310,7 +9337,7 @@
         <v>0.62697505292422928</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>8.1999999999999993</v>
       </c>
@@ -9319,7 +9346,7 @@
         <v>0.66821789367236439</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>8.3000000000000007</v>
       </c>
@@ -9328,7 +9355,7 @@
         <v>0.70951397091120683</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>8.4</v>
       </c>
@@ -9337,7 +9364,7 @@
         <v>0.75086232538105602</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>8.5</v>
       </c>
@@ -9346,7 +9373,7 @@
         <v>0.79226202628867481</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>8.6</v>
       </c>
@@ -9355,7 +9382,7 @@
         <v>0.83371217013848176</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>8.6999999999999993</v>
       </c>
@@ -9364,7 +9391,7 @@
         <v>0.87521187962473723</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>8.8000000000000007</v>
       </c>
@@ -9373,7 +9400,7 @@
         <v>0.91676030258086794</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>8.9</v>
       </c>
@@ -9382,7 +9409,7 @@
         <v>0.95835661098237068</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>9</v>
       </c>
@@ -9400,20 +9427,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -9433,182 +9460,182 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
         <f ca="1">SUM(B4:B6)</f>
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:E3" ca="1" si="0">SUM(C4:C6)</f>
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F3">
         <f ca="1">SUM(B3:E3)</f>
-        <v>217</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
         <f ca="1">RANDBETWEEN(1,50)</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:E6" ca="1" si="1">RANDBETWEEN(1,50)</f>
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <f ca="1">SUM(B4:E4)</f>
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
         <f t="shared" ref="B5:B6" ca="1" si="2">RANDBETWEEN(1,50)</f>
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5:F6" ca="1" si="3">SUM(B5:E5)</f>
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="3"/>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
         <f ca="1">B4*VLOOKUP($A$4,$C$21:$F$24,2,FALSE)+B5*VLOOKUP($A$5,$C$21:$F$24,2,FALSE)+B6*VLOOKUP($A$6,$C$21:$F$24,2,FALSE)</f>
-        <v>619750</v>
+        <v>1320790</v>
       </c>
       <c r="C8">
         <f t="shared" ref="C8:F8" ca="1" si="4">C4*VLOOKUP($A$4,$C$21:$F$24,2,FALSE)+C5*VLOOKUP($A$5,$C$21:$F$24,2,FALSE)+C6*VLOOKUP($A$6,$C$21:$F$24,2,FALSE)</f>
-        <v>831550</v>
+        <v>786540</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="4"/>
-        <v>305190</v>
+        <v>620200</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="4"/>
-        <v>1231240</v>
+        <v>1433260</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="4"/>
-        <v>2987730</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4160790</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
         <f ca="1">B4*VLOOKUP($A$4,$C$21:$F$24,4,FALSE)+B5*VLOOKUP($A$5,$C$21:$F$24,4,FALSE)+B6*VLOOKUP($A$6,$C$21:$F$24,4,FALSE)</f>
-        <v>460449.20000000007</v>
+        <v>1011204</v>
       </c>
       <c r="C9">
         <f t="shared" ref="C9:F9" ca="1" si="5">C4*VLOOKUP($A$4,$C$21:$F$24,4,FALSE)+C5*VLOOKUP($A$5,$C$21:$F$24,4,FALSE)+C6*VLOOKUP($A$6,$C$21:$F$24,4,FALSE)</f>
-        <v>634341.80000000005</v>
+        <v>576238.80000000005</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="5"/>
-        <v>227346</v>
+        <v>471711.4</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="5"/>
-        <v>907743.60000000009</v>
+        <v>1087726.8</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="5"/>
-        <v>2229880.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3146881</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
         <f ca="1">B8-B9</f>
-        <v>159300.79999999993</v>
+        <v>309586</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:F10" ca="1" si="6">C8-C9</f>
-        <v>197208.19999999995</v>
+        <v>210301.19999999995</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="6"/>
-        <v>77844</v>
+        <v>148488.59999999998</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="6"/>
-        <v>323496.39999999991</v>
+        <v>345533.19999999995</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="6"/>
-        <v>757849.39999999991</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1013909</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -9629,32 +9656,32 @@
         <v>40006</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <f ca="1">$A$22*B8</f>
-        <v>1549.375</v>
+        <v>3301.9749999999999</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:F13" ca="1" si="7">$A$22*C8</f>
-        <v>2078.875</v>
+        <f t="shared" ref="C13:E13" ca="1" si="7">$A$22*C8</f>
+        <v>1966.3500000000001</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="7"/>
-        <v>762.97500000000002</v>
+        <v>1550.5</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="7"/>
-        <v>3078.1</v>
+        <v>3583.15</v>
       </c>
       <c r="F13">
         <f ca="1">$A$22*F8</f>
-        <v>7469.3249999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10401.975</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -9675,107 +9702,107 @@
         <v>88006</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
         <f ca="1">B8*$A$24</f>
-        <v>111555</v>
+        <v>237742.19999999998</v>
       </c>
       <c r="C15">
         <f t="shared" ref="C15:F15" ca="1" si="8">C8*$A$24</f>
-        <v>149679</v>
+        <v>141577.19999999998</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="8"/>
-        <v>54934.2</v>
+        <v>111636</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="8"/>
-        <v>221623.19999999998</v>
+        <v>257986.8</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="8"/>
-        <v>537791.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>748942.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
         <f ca="1">SUM(B12:B15)</f>
-        <v>145104.375</v>
+        <v>273044.17499999999</v>
       </c>
       <c r="C16">
         <f t="shared" ref="C16:F16" ca="1" si="9">SUM(C12:C15)</f>
-        <v>183759.875</v>
+        <v>175545.55</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="9"/>
-        <v>87701.174999999988</v>
+        <v>145190.5</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="9"/>
-        <v>256707.3</v>
+        <v>293575.95</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="9"/>
-        <v>673272.72500000009</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>887356.17499999993</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
         <f ca="1">B10-B16</f>
-        <v>14196.42499999993</v>
+        <v>36541.825000000012</v>
       </c>
       <c r="C18">
         <f t="shared" ref="C18:F18" ca="1" si="10">C10-C16</f>
-        <v>13448.324999999953</v>
+        <v>34755.649999999965</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="10"/>
-        <v>-9857.1749999999884</v>
+        <v>3298.0999999999767</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="10"/>
-        <v>66789.099999999919</v>
+        <v>51957.249999999942</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="10"/>
-        <v>84576.674999999814</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>126552.82500000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19">
         <f ca="1">B18/B8</f>
-        <v>2.2906696248487179E-2</v>
+        <v>2.766664269111669E-2</v>
       </c>
       <c r="C19">
         <f t="shared" ref="C19:F19" ca="1" si="11">C18/C8</f>
-        <v>1.6172599362635987E-2</v>
+        <v>4.4188026038090834E-2</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="11"/>
-        <v>-3.2298486188931448E-2</v>
+        <v>5.3178007094485278E-3</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="11"/>
-        <v>5.4245394886455862E-2</v>
+        <v>3.6251098893431713E-2</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="11"/>
-        <v>2.8308004739384017E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.0415576128571754E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -9786,7 +9813,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -9803,7 +9830,7 @@
         <v>7552.8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -9820,7 +9847,7 @@
         <v>10870.6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="3">
         <v>0.18</v>
       </c>

</xml_diff>